<commit_message>
Muda Excel e adiciona txt
</commit_message>
<xml_diff>
--- a/Excel_teste.xlsx
+++ b/Excel_teste.xlsx
@@ -349,10 +349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,6 +574,226 @@
         <v>0.61753049889877276</v>
       </c>
       <c r="C20">
+        <v>4.8979382382076109E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>9.5586362156384164E-2</v>
+      </c>
+      <c r="B21">
+        <v>0.43014567904895973</v>
+      </c>
+      <c r="C21">
+        <v>0.93475123691792272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.58498545186059103</v>
+      </c>
+      <c r="B22">
+        <v>0.83315731204136279</v>
+      </c>
+      <c r="C22">
+        <v>0.30925153574537789</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.25411504559554809</v>
+      </c>
+      <c r="B23">
+        <v>0.69160138448215147</v>
+      </c>
+      <c r="C23">
+        <v>0.7604975177012897</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.16805844861551922</v>
+      </c>
+      <c r="B24">
+        <v>0.22811306315321656</v>
+      </c>
+      <c r="C24">
+        <v>0.69161502623442972</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.6102277376579327</v>
+      </c>
+      <c r="B25">
+        <v>0.3936799543107754</v>
+      </c>
+      <c r="C25">
+        <v>0.43110966795358363</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.94967521092361362</v>
+      </c>
+      <c r="B26">
+        <v>0.92650611657540438</v>
+      </c>
+      <c r="C26">
+        <v>0.11818201202586232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.92445976167215416</v>
+      </c>
+      <c r="B27">
+        <v>0.60888576552908402</v>
+      </c>
+      <c r="C27">
+        <v>0.70253596673549734</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.42424387436649103</v>
+      </c>
+      <c r="B28">
+        <v>9.5833939854706895E-2</v>
+      </c>
+      <c r="C28">
+        <v>0.12564639228445462</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.64888705191147122</v>
+      </c>
+      <c r="B29">
+        <v>0.67748627042370269</v>
+      </c>
+      <c r="C29">
+        <v>0.21943385355532774</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.95988685072404034</v>
+      </c>
+      <c r="B30">
+        <v>0.77084439638157165</v>
+      </c>
+      <c r="C30">
+        <v>0.24509829978459619</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.2546894194395577</v>
+      </c>
+      <c r="B31">
+        <v>0.72123200739599824</v>
+      </c>
+      <c r="C31">
+        <v>0.54051811044464204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.23232590780878914</v>
+      </c>
+      <c r="B32">
+        <v>0.56979267886314988</v>
+      </c>
+      <c r="C32">
+        <v>0.96074787332329536</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.43591726258290364</v>
+      </c>
+      <c r="B33">
+        <v>0.48496244984527692</v>
+      </c>
+      <c r="C33">
+        <v>0.81742098941475949</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0.97660202975084276</v>
+      </c>
+      <c r="B34">
+        <v>0.3795805588922665</v>
+      </c>
+      <c r="C34">
+        <v>0.72088073900086425</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.99068217148084081</v>
+      </c>
+      <c r="B35">
+        <v>0.80295788433314919</v>
+      </c>
+      <c r="C35">
+        <v>0.25989262000867286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0.25321974100165023</v>
+      </c>
+      <c r="B36">
+        <v>0.34481406734776798</v>
+      </c>
+      <c r="C36">
+        <v>0.852821021292405</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0.55984252571216242</v>
+      </c>
+      <c r="B37">
+        <v>0.90623904081576701</v>
+      </c>
+      <c r="C37">
+        <v>0.90774857717611734</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>8.4129693539714112E-2</v>
+      </c>
+      <c r="B38">
+        <v>0.70510070534744218</v>
+      </c>
+      <c r="C38">
+        <v>3.1123204474163835E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0.17190784462471487</v>
+      </c>
+      <c r="B39">
+        <v>0.21863297632249701</v>
+      </c>
+      <c r="C39">
+        <v>4.0217534694793833E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0.26502759355714556</v>
+      </c>
+      <c r="B40">
+        <v>0.61753049889877276</v>
+      </c>
+      <c r="C40">
         <v>4.8979382382076109E-3</v>
       </c>
     </row>

</xml_diff>